<commit_message>
Actualizar del cronograma - Hito 1 (100%)
</commit_message>
<xml_diff>
--- a/Desarrollo/SGC/Gestion/Cronograma.xlsx
+++ b/Desarrollo/SGC/Gestion/Cronograma.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronald\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTO\FisiDev-Solutions\Desarrollo\SGC\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85AE158-30A8-4799-BEFA-B66BF6393F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="2550" windowWidth="17085" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10020" yWindow="2550" windowWidth="17085" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="CRONOGRAMA" sheetId="1" r:id="rId1"/>
@@ -225,8 +224,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,7 +770,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="CRONOGRAMA-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="CRONOGRAMA-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="3"/>
       <tableStyleElement type="firstRowStripe" dxfId="2"/>
       <tableStyleElement type="secondRowStripe" dxfId="1"/>
@@ -796,15 +795,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CRONOGRAMA_DE_ACTIVIDADES" displayName="CRONOGRAMA_DE_ACTIVIDADES" ref="A1:G19" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CRONOGRAMA_DE_ACTIVIDADES" displayName="CRONOGRAMA_DE_ACTIVIDADES" ref="A1:G19" headerRowDxfId="0">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ARTEFACTO"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NOMENCLATURA"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ROL"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="INICIO"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FIN"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ESTADO"/>
+    <tableColumn id="1" name="Tarea"/>
+    <tableColumn id="2" name="ARTEFACTO"/>
+    <tableColumn id="3" name="NOMENCLATURA"/>
+    <tableColumn id="4" name="ROL"/>
+    <tableColumn id="5" name="INICIO"/>
+    <tableColumn id="6" name="FIN"/>
+    <tableColumn id="7" name="ESTADO"/>
   </tableColumns>
   <tableStyleInfo name="CRONOGRAMA-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1007,7 +1006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1015,10 +1014,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1"/>
@@ -1029,7 +1028,7 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1099,7 +1098,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="34" t="s">
         <v>54</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
@@ -1186,10 +1185,10 @@
         <v>45785</v>
       </c>
       <c r="G7" s="30">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="20" t="s">
         <v>22</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>26</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="35" t="s">
         <v>55</v>
       </c>
@@ -1258,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="15" t="s">
         <v>33</v>
       </c>
@@ -1302,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="20" t="s">
         <v>37</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="24" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="20" t="s">
         <v>45</v>
       </c>
@@ -1394,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="24" t="s">
         <v>48</v>
       </c>
@@ -1417,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="20" t="s">
         <v>51</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" s="45" t="s">
         <v>58</v>
       </c>
@@ -1455,16 +1454,16 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A11:A19 A2:D7 B8:D19 A8:A9" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G7 G8:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A11:A19 A2:D7 B8:D19 A8:A9"/>
+    <dataValidation type="list" allowBlank="1" sqref="G2:G7 G8:G19">
       <formula1>"Sin comenzar,En curso,Bloqueado,Completado"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F7 E8:F19" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F7 E8:F19">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
añadimos FeedBack del usuario
</commit_message>
<xml_diff>
--- a/Desarrollo/SGC/Gestion/Cronograma.xlsx
+++ b/Desarrollo/SGC/Gestion/Cronograma.xlsx
@@ -225,7 +225,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,12 +1010,12 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1"/>
@@ -1026,7 +1026,7 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>54</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>22</v>
       </c>
@@ -1206,10 +1206,10 @@
         <v>45778</v>
       </c>
       <c r="G8" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>26</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>55</v>
       </c>
@@ -1252,10 +1252,10 @@
         <v>45789</v>
       </c>
       <c r="G10" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
@@ -1275,10 +1275,10 @@
         <v>45790</v>
       </c>
       <c r="G11" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>33</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>34</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>37</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>41</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>45</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>48</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>51</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
actualizacion en el cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/SGC/Gestion/Cronograma.xlsx
+++ b/Desarrollo/SGC/Gestion/Cronograma.xlsx
@@ -225,7 +225,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,12 +1010,12 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1"/>
@@ -1026,7 +1026,7 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="33" t="s">
         <v>54</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>22</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="22" t="s">
         <v>26</v>
       </c>
@@ -1229,10 +1229,10 @@
         <v>45781</v>
       </c>
       <c r="G9" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="34" t="s">
         <v>55</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>33</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>34</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>37</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="23" t="s">
         <v>41</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>45</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>48</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>51</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" s="44" t="s">
         <v>58</v>
       </c>

</xml_diff>